<commit_message>
Update baselines: ground truth and test data
</commit_message>
<xml_diff>
--- a/baselines.xlsx
+++ b/baselines.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quert/Documents/GitHub/acl-research/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quert/Documents/GitHub/KGG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5483E46-A9FE-CE45-A826-36728F545719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6B34D4-F054-564A-BE4E-20638DBC0A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{9DDA97F0-446E-8741-84E0-45819061BEAD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>ROUGE-1</t>
   </si>
@@ -81,6 +81,21 @@
   </si>
   <si>
     <t>MEDIAN</t>
+  </si>
+  <si>
+    <t>Ground Truth (all)</t>
+  </si>
+  <si>
+    <t>Ground Truth (Test Set)</t>
+  </si>
+  <si>
+    <t>BLEU-4</t>
+  </si>
+  <si>
+    <t>GPT-3.5</t>
+  </si>
+  <si>
+    <t>GPT-3.5 (length restricted)</t>
   </si>
 </sst>
 </file>
@@ -89,7 +104,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -153,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -165,10 +180,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -485,15 +507,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21CFAA03-9A7E-9E47-88B5-AB72ED5F4100}">
-  <dimension ref="C1:J8"/>
+  <dimension ref="B1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="166" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -503,7 +529,7 @@
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
     </row>
-    <row r="2" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
@@ -522,92 +548,164 @@
       <c r="H2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C3" s="4">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="D3" s="5">
+        <v>1.6E-2</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0.1232</v>
+      </c>
+      <c r="F3" s="5">
+        <v>7.6600000000000001E-2</v>
+      </c>
+      <c r="G3" s="5">
+        <v>1.44E-2</v>
+      </c>
+      <c r="H3" s="5">
+        <v>4.3E-3</v>
+      </c>
+      <c r="I3" s="9">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.14030000000000001</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1.67E-2</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0.1235</v>
+      </c>
+      <c r="F4" s="5">
+        <v>7.7100000000000002E-2</v>
+      </c>
+      <c r="G4" s="5">
+        <v>1.52E-2</v>
+      </c>
+      <c r="H4" s="5">
+        <v>4.4000000000000003E-3</v>
+      </c>
+      <c r="I4" s="9">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="4">
         <v>7.9699999999999993E-2</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D5" s="4">
         <v>7.1999999999999998E-3</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E5" s="4">
         <v>7.2700000000000001E-2</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F5" s="4">
         <v>3.56E-2</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G5" s="4">
         <v>3.7000000000000002E-3</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H5" s="4">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4">
+      <c r="I5" s="5">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4">
         <v>0.80189999999999995</v>
       </c>
     </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C6" s="1" t="s">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C7" s="4" t="s">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D11" s="4">
         <v>1</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E11" s="5">
         <v>292.94619999999998</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F11" s="4">
         <v>473</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G11" s="6">
         <v>296</v>
       </c>
     </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C8" s="4" t="s">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D12" s="4">
         <v>7</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E12" s="5">
         <v>34.664200000000001</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F12" s="4">
         <v>140</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G12" s="6">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update hand-selected examples and scores
</commit_message>
<xml_diff>
--- a/baselines.xlsx
+++ b/baselines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quert/Documents/GitHub/KGG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F5D8D5-8F15-7A43-8C63-AFA898A999B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B147CE7-E37E-A642-8AFA-4F681B8EE08C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{9DDA97F0-446E-8741-84E0-45819061BEAD}"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{9DDA97F0-446E-8741-84E0-45819061BEAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="32">
   <si>
     <t>ROUGE-1</t>
   </si>
@@ -102,6 +102,36 @@
   </si>
   <si>
     <t>All</t>
+  </si>
+  <si>
+    <t>Inputs - Reference</t>
+  </si>
+  <si>
+    <t>GPT-3.5 - Reference</t>
+  </si>
+  <si>
+    <t>GPT-4 - Reference</t>
+  </si>
+  <si>
+    <t>GPT-3.5 - Inputs</t>
+  </si>
+  <si>
+    <t>GPT-4 - Inputs</t>
+  </si>
+  <si>
+    <t>Example 1</t>
+  </si>
+  <si>
+    <t>Example 2</t>
+  </si>
+  <si>
+    <t>Example 3</t>
+  </si>
+  <si>
+    <t>Example 4</t>
+  </si>
+  <si>
+    <t>Example 5</t>
   </si>
 </sst>
 </file>
@@ -112,7 +142,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -132,6 +162,12 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -174,8 +210,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -193,10 +232,16 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,206 +556,1124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21CFAA03-9A7E-9E47-88B5-AB72ED5F4100}">
-  <dimension ref="B1:K12"/>
+  <dimension ref="B1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="166" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.6640625" customWidth="1"/>
     <col min="2" max="2" width="23.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
         <v>0.13900000000000001</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="4">
         <v>1.6E-2</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="4">
         <v>0.1232</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="4">
         <v>7.6600000000000001E-2</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="4">
         <v>1.44E-2</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="4">
         <v>4.3E-3</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="8">
         <v>1.6999999999999999E-3</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
         <v>7.9699999999999993E-2</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="3">
         <v>7.1999999999999998E-3</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="3">
         <v>7.2700000000000001E-2</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="3">
         <v>3.56E-2</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="3">
         <v>3.7000000000000002E-3</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="3">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="4">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2">
+      <c r="J4" s="3"/>
+      <c r="K4" s="3">
         <v>0.80189999999999995</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
+      <c r="C5" s="4">
+        <v>0.1651</v>
+      </c>
+      <c r="D5" s="4">
+        <v>3.8699999999999998E-2</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.1032</v>
+      </c>
+      <c r="F5" s="4">
+        <v>8.0299999999999996E-2</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1.5699999999999999E-2</v>
+      </c>
+      <c r="H5" s="4">
+        <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="I5" s="8">
+        <v>1.9E-3</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4">
+        <v>0.83</v>
+      </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
+      <c r="C6" s="4">
+        <v>0.159</v>
+      </c>
+      <c r="D6" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.1135</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.10290000000000001</v>
+      </c>
+      <c r="G6" s="4">
+        <v>2.8E-3</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="I6" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="J6" s="6"/>
+      <c r="K6" s="3">
+        <v>0.83689999999999998</v>
+      </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="10" t="s">
         <v>19</v>
       </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="3">
         <v>1</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="4">
         <v>292.94619999999998</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="3">
         <v>473</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="5">
         <v>296</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="3">
         <v>7</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="4">
         <v>34.664200000000001</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="3">
         <v>140</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="5">
         <v>29</v>
       </c>
     </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B15" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B16" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.31940000000000002</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.1069</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.18160000000000001</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0.27160000000000001</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.1139</v>
+      </c>
+      <c r="H16" s="1">
+        <v>3.1699999999999999E-2</v>
+      </c>
+      <c r="I16" s="1">
+        <v>1.4800000000000001E-2</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0.83689999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B17" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.43209999999999998</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.1651</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0.18820000000000001</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0.18129999999999999</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0.113</v>
+      </c>
+      <c r="H17" s="3">
+        <v>5.91E-2</v>
+      </c>
+      <c r="I17" s="3">
+        <v>3.95E-2</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0.8417</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B18" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0.45729999999999998</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.19239999999999999</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0.2024</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0.31979999999999997</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0.17480000000000001</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="I18" s="3">
+        <v>5.74E-2</v>
+      </c>
+      <c r="J18" s="3">
+        <v>0.8569</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B19" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.2233</v>
+      </c>
+      <c r="D19" s="3">
+        <v>5.0099999999999999E-2</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0.15620000000000001</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0.2034</v>
+      </c>
+      <c r="G19" s="3">
+        <v>6.3899999999999998E-2</v>
+      </c>
+      <c r="H19" s="3">
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="I19" s="3">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J19" s="3">
+        <v>0.8105</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B20" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.18540000000000001</v>
+      </c>
+      <c r="D20" s="3">
+        <v>4.6100000000000002E-2</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0.1196</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0.29549999999999998</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0.1179</v>
+      </c>
+      <c r="H20" s="3">
+        <v>3.6700000000000003E-2</v>
+      </c>
+      <c r="I20" s="3">
+        <v>4.1000000000000003E-3</v>
+      </c>
+      <c r="J20" s="3">
+        <v>0.81730000000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B23" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B24" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.48949999999999999</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0.16520000000000001</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0.1489</v>
+      </c>
+      <c r="G24" s="1">
+        <v>6.13E-2</v>
+      </c>
+      <c r="H24" s="1">
+        <v>1.7299999999999999E-2</v>
+      </c>
+      <c r="I24" s="1">
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0.83560000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B25" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0.46289999999999998</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0.21490000000000001</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0.1948</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0.3498</v>
+      </c>
+      <c r="G25" s="3">
+        <v>0.2298</v>
+      </c>
+      <c r="H25" s="3">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="I25" s="3">
+        <v>8.4400000000000003E-2</v>
+      </c>
+      <c r="J25" s="3">
+        <v>0.85260000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B26" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0.38069999999999998</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0.17460000000000001</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0.15529999999999999</v>
+      </c>
+      <c r="F26" s="3">
+        <v>0.33829999999999999</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0.20380000000000001</v>
+      </c>
+      <c r="H26" s="3">
+        <v>0.10979999999999999</v>
+      </c>
+      <c r="I26" s="3">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="J26" s="3">
+        <v>0.84360000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B27" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0.39810000000000001</v>
+      </c>
+      <c r="D27" s="3">
+        <v>7.2800000000000004E-2</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0.14990000000000001</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0.1981</v>
+      </c>
+      <c r="G27" s="3">
+        <v>4.6600000000000003E-2</v>
+      </c>
+      <c r="H27" s="3">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="I27" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="J27" s="3">
+        <v>0.81579999999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B28" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0.38940000000000002</v>
+      </c>
+      <c r="D28" s="3">
+        <v>7.6100000000000001E-2</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0.15679999999999999</v>
+      </c>
+      <c r="F28" s="3">
+        <v>0.2218</v>
+      </c>
+      <c r="G28" s="3">
+        <v>4.9099999999999998E-2</v>
+      </c>
+      <c r="H28" s="3">
+        <v>3.8E-3</v>
+      </c>
+      <c r="I28" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="J28" s="3">
+        <v>0.81779999999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B31" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B32" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0.42109999999999997</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0.12770000000000001</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0.27560000000000001</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0.19159999999999999</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H32" s="1">
+        <v>3.2399999999999998E-2</v>
+      </c>
+      <c r="I32" s="1">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="J32" s="1">
+        <v>0.81559999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B33" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="3">
+        <v>0.38540000000000002</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0.1867</v>
+      </c>
+      <c r="E33" s="3">
+        <v>0.2009</v>
+      </c>
+      <c r="F33" s="3">
+        <v>0.31709999999999999</v>
+      </c>
+      <c r="G33" s="3">
+        <v>0.18179999999999999</v>
+      </c>
+      <c r="H33" s="3">
+        <v>0.1018</v>
+      </c>
+      <c r="I33" s="3">
+        <v>5.9900000000000002E-2</v>
+      </c>
+      <c r="J33" s="3">
+        <v>0.84909999999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B34" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="3">
+        <v>0.37409999999999999</v>
+      </c>
+      <c r="D34" s="3">
+        <v>0.13370000000000001</v>
+      </c>
+      <c r="E34" s="3">
+        <v>0.19919999999999999</v>
+      </c>
+      <c r="F34" s="3">
+        <v>0.34720000000000001</v>
+      </c>
+      <c r="G34" s="3">
+        <v>0.1326</v>
+      </c>
+      <c r="H34" s="3">
+        <v>4.1799999999999997E-2</v>
+      </c>
+      <c r="I34" s="3">
+        <v>1.9099999999999999E-2</v>
+      </c>
+      <c r="J34" s="3">
+        <v>0.85250000000000004</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B35" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="3">
+        <v>0.2661</v>
+      </c>
+      <c r="D35" s="3">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="E35" s="3">
+        <v>0.18720000000000001</v>
+      </c>
+      <c r="F35" s="3">
+        <v>0.22650000000000001</v>
+      </c>
+      <c r="G35" s="3">
+        <v>7.6899999999999996E-2</v>
+      </c>
+      <c r="H35" s="3">
+        <v>1.0500000000000001E-2</v>
+      </c>
+      <c r="I35" s="3">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="J35" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B36" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" s="3">
+        <v>0.30409999999999998</v>
+      </c>
+      <c r="D36" s="3">
+        <v>7.7600000000000002E-2</v>
+      </c>
+      <c r="E36" s="3">
+        <v>0.19450000000000001</v>
+      </c>
+      <c r="F36" s="3">
+        <v>0.29809999999999998</v>
+      </c>
+      <c r="G36" s="3">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="H36" s="3">
+        <v>1.52E-2</v>
+      </c>
+      <c r="I36" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="J36" s="3">
+        <v>0.80800000000000005</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B38" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B39" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" s="1">
+        <v>0.41110000000000002</v>
+      </c>
+      <c r="D39" s="1">
+        <v>9.4799999999999995E-2</v>
+      </c>
+      <c r="E39" s="1">
+        <v>0.3196</v>
+      </c>
+      <c r="F39" s="1">
+        <v>0.19650000000000001</v>
+      </c>
+      <c r="G39" s="1">
+        <v>7.5300000000000006E-2</v>
+      </c>
+      <c r="H39" s="1">
+        <v>1.7399999999999999E-2</v>
+      </c>
+      <c r="I39" s="1">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="J39" s="1">
+        <v>0.82540000000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B40" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40" s="3">
+        <v>0.41489999999999999</v>
+      </c>
+      <c r="D40" s="3">
+        <v>0.16350000000000001</v>
+      </c>
+      <c r="E40" s="3">
+        <v>0.26740000000000003</v>
+      </c>
+      <c r="F40" s="3">
+        <v>0.2596</v>
+      </c>
+      <c r="G40" s="3">
+        <v>0.15659999999999999</v>
+      </c>
+      <c r="H40" s="3">
+        <v>9.1800000000000007E-2</v>
+      </c>
+      <c r="I40" s="3">
+        <v>6.0499999999999998E-2</v>
+      </c>
+      <c r="J40" s="3">
+        <v>0.84230000000000005</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B41" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C41" s="3">
+        <v>0.42</v>
+      </c>
+      <c r="D41" s="3">
+        <v>0.1239</v>
+      </c>
+      <c r="E41" s="3">
+        <v>0.23949999999999999</v>
+      </c>
+      <c r="F41" s="3">
+        <v>0.3377</v>
+      </c>
+      <c r="G41" s="3">
+        <v>0.13289999999999999</v>
+      </c>
+      <c r="H41" s="3">
+        <v>6.6699999999999995E-2</v>
+      </c>
+      <c r="I41" s="3">
+        <v>3.6799999999999999E-2</v>
+      </c>
+      <c r="J41" s="3">
+        <v>0.84289999999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B42" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" s="3">
+        <v>0.3594</v>
+      </c>
+      <c r="D42" s="3">
+        <v>0.1046</v>
+      </c>
+      <c r="E42" s="3">
+        <v>0.27629999999999999</v>
+      </c>
+      <c r="F42" s="3">
+        <v>0.17549999999999999</v>
+      </c>
+      <c r="G42" s="3">
+        <v>7.7100000000000002E-2</v>
+      </c>
+      <c r="H42" s="3">
+        <v>2.4199999999999999E-2</v>
+      </c>
+      <c r="I42" s="3">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="J42" s="3">
+        <v>0.81220000000000003</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B43" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C43" s="3">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="D43" s="3">
+        <v>7.5600000000000001E-2</v>
+      </c>
+      <c r="E43" s="3">
+        <v>0.25280000000000002</v>
+      </c>
+      <c r="F43" s="3">
+        <v>0.25169999999999998</v>
+      </c>
+      <c r="G43" s="3">
+        <v>6.3100000000000003E-2</v>
+      </c>
+      <c r="H43" s="3">
+        <v>6.7000000000000002E-3</v>
+      </c>
+      <c r="I43" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="J43" s="3">
+        <v>0.81379999999999997</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B45" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I45" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B46" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C46" s="1">
+        <v>0.44919999999999999</v>
+      </c>
+      <c r="D46" s="1">
+        <v>0.1716</v>
+      </c>
+      <c r="E46" s="1">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="F46" s="1">
+        <v>0.23830000000000001</v>
+      </c>
+      <c r="G46" s="1">
+        <v>0.123</v>
+      </c>
+      <c r="H46" s="1">
+        <v>3.9600000000000003E-2</v>
+      </c>
+      <c r="I46" s="1">
+        <v>1.6199999999999999E-2</v>
+      </c>
+      <c r="J46" s="1">
+        <v>0.82899999999999996</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B47" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47" s="3">
+        <v>0.44740000000000002</v>
+      </c>
+      <c r="D47" s="3">
+        <v>0.19350000000000001</v>
+      </c>
+      <c r="E47" s="3">
+        <v>0.33079999999999998</v>
+      </c>
+      <c r="F47" s="3">
+        <v>0.27</v>
+      </c>
+      <c r="G47" s="3">
+        <v>0.1454</v>
+      </c>
+      <c r="H47" s="3">
+        <v>7.7899999999999997E-2</v>
+      </c>
+      <c r="I47" s="3">
+        <v>4.7899999999999998E-2</v>
+      </c>
+      <c r="J47" s="3">
+        <v>0.83909999999999996</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B48" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C48" s="3">
+        <v>0.3226</v>
+      </c>
+      <c r="D48" s="3">
+        <v>0.1062</v>
+      </c>
+      <c r="E48" s="3">
+        <v>0.21890000000000001</v>
+      </c>
+      <c r="F48" s="3">
+        <v>0.30640000000000001</v>
+      </c>
+      <c r="G48" s="3">
+        <v>7.6899999999999996E-2</v>
+      </c>
+      <c r="H48" s="3">
+        <v>1.72E-2</v>
+      </c>
+      <c r="I48" s="3">
+        <v>4.3E-3</v>
+      </c>
+      <c r="J48" s="3">
+        <v>0.82299999999999995</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B49" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C49" s="3">
+        <v>0.3301</v>
+      </c>
+      <c r="D49" s="3">
+        <v>9.3299999999999994E-2</v>
+      </c>
+      <c r="E49" s="3">
+        <v>0.2288</v>
+      </c>
+      <c r="F49" s="3">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="G49" s="3">
+        <v>6.7699999999999996E-2</v>
+      </c>
+      <c r="H49" s="3">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="I49" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="J49" s="3">
+        <v>0.80810000000000004</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B50" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C50" s="3">
+        <v>0.2215</v>
+      </c>
+      <c r="D50" s="3">
+        <v>3.44E-2</v>
+      </c>
+      <c r="E50" s="3">
+        <v>0.1638</v>
+      </c>
+      <c r="F50" s="3">
+        <v>0.26379999999999998</v>
+      </c>
+      <c r="G50" s="3">
+        <v>2.1399999999999999E-2</v>
+      </c>
+      <c r="H50" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="I50" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="J50" s="3">
+        <v>0.80369999999999997</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add concept and human-selected test
</commit_message>
<xml_diff>
--- a/baselines.xlsx
+++ b/baselines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quert/Documents/GitHub/KGG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B147CE7-E37E-A642-8AFA-4F681B8EE08C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82A06DA-3325-A846-A40F-37EFFE47987E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{9DDA97F0-446E-8741-84E0-45819061BEAD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{9DDA97F0-446E-8741-84E0-45819061BEAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="34">
   <si>
     <t>ROUGE-1</t>
   </si>
@@ -132,17 +132,24 @@
   </si>
   <si>
     <t>Example 5</t>
+  </si>
+  <si>
+    <t>zero-shot (modified prompt)</t>
+  </si>
+  <si>
+    <t>few-shot (modified prompt)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="170" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -168,6 +175,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -210,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -242,6 +262,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,16 +591,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21CFAA03-9A7E-9E47-88B5-AB72ED5F4100}">
-  <dimension ref="B1:K50"/>
+  <dimension ref="B1:K66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="J50" sqref="J50"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="150" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23.83203125" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="16.83203125" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" customWidth="1"/>
@@ -1671,6 +1706,300 @@
         <v>0.80369999999999997</v>
       </c>
     </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B52" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B53" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D53" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E53" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F53" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="G53" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="H53" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="I53" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="J53" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B54" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C54" s="20">
+        <v>0.26029999999999998</v>
+      </c>
+      <c r="D54" s="20">
+        <v>8.14E-2</v>
+      </c>
+      <c r="E54" s="20">
+        <v>0.1512</v>
+      </c>
+      <c r="F54" s="20">
+        <v>0.29859999999999998</v>
+      </c>
+      <c r="G54" s="20">
+        <v>0.1016</v>
+      </c>
+      <c r="H54" s="20">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="I54" s="20">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="J54" s="19">
+        <v>0.83199999999999996</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B55" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C55" s="20"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="20"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="20"/>
+      <c r="H55" s="20"/>
+      <c r="I55" s="20"/>
+      <c r="J55" s="19"/>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B56" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C56" s="20">
+        <v>0.39</v>
+      </c>
+      <c r="D56" s="20">
+        <v>9.4100000000000003E-2</v>
+      </c>
+      <c r="E56" s="20">
+        <v>0.19059999999999999</v>
+      </c>
+      <c r="F56" s="20">
+        <v>0.2112</v>
+      </c>
+      <c r="G56" s="20">
+        <v>8.1299999999999997E-2</v>
+      </c>
+      <c r="H56" s="20">
+        <v>5.3199999999999997E-2</v>
+      </c>
+      <c r="I56" s="20">
+        <v>4.2700000000000002E-2</v>
+      </c>
+      <c r="J56" s="19">
+        <v>0.81200000000000006</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B57" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C57" s="20"/>
+      <c r="D57" s="20"/>
+      <c r="E57" s="20"/>
+      <c r="F57" s="20"/>
+      <c r="G57" s="20"/>
+      <c r="H57" s="20"/>
+      <c r="I57" s="20"/>
+      <c r="J57" s="19"/>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B58" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C58" s="20">
+        <v>0.19139999999999999</v>
+      </c>
+      <c r="D58" s="20">
+        <v>3.2300000000000002E-2</v>
+      </c>
+      <c r="E58" s="20">
+        <v>0.1183</v>
+      </c>
+      <c r="F58" s="20">
+        <v>0.27460000000000001</v>
+      </c>
+      <c r="G58" s="20">
+        <v>6.3600000000000004E-2</v>
+      </c>
+      <c r="H58" s="20">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="I58" s="20">
+        <v>1E-4</v>
+      </c>
+      <c r="J58" s="19">
+        <v>0.80400000000000005</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B60" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B61" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C61" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D61" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E61" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F61" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="G61" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="H61" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="I61" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="J61" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B62" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C62" s="20">
+        <v>0.26029999999999998</v>
+      </c>
+      <c r="D62" s="20">
+        <v>8.14E-2</v>
+      </c>
+      <c r="E62" s="20">
+        <v>0.1512</v>
+      </c>
+      <c r="F62" s="20">
+        <v>0.29859999999999998</v>
+      </c>
+      <c r="G62" s="20">
+        <v>0.1016</v>
+      </c>
+      <c r="H62" s="20">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="I62" s="20">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="J62" s="21">
+        <v>0.83199999999999996</v>
+      </c>
+    </row>
+    <row r="63" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B63" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C63" s="20"/>
+      <c r="D63" s="20"/>
+      <c r="E63" s="20"/>
+      <c r="F63" s="20"/>
+      <c r="G63" s="20"/>
+      <c r="H63" s="20"/>
+      <c r="I63" s="20"/>
+      <c r="J63" s="21"/>
+    </row>
+    <row r="64" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B64" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C64" s="20">
+        <v>0.217</v>
+      </c>
+      <c r="D64" s="20">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="E64" s="20">
+        <v>0.1239</v>
+      </c>
+      <c r="F64" s="20">
+        <v>0.20119999999999999</v>
+      </c>
+      <c r="G64" s="20">
+        <v>7.8899999999999998E-2</v>
+      </c>
+      <c r="H64" s="20">
+        <v>3.2300000000000002E-2</v>
+      </c>
+      <c r="I64" s="20">
+        <v>2.06E-2</v>
+      </c>
+      <c r="J64" s="21">
+        <v>0.81020000000000003</v>
+      </c>
+    </row>
+    <row r="65" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B65" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C65" s="20"/>
+      <c r="D65" s="20"/>
+      <c r="E65" s="20"/>
+      <c r="F65" s="20"/>
+      <c r="G65" s="20"/>
+      <c r="H65" s="20"/>
+      <c r="I65" s="20"/>
+      <c r="J65" s="21"/>
+    </row>
+    <row r="66" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B66" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C66" s="20">
+        <v>0.217</v>
+      </c>
+      <c r="D66" s="20">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="E66" s="20">
+        <v>0.12379999999999999</v>
+      </c>
+      <c r="F66" s="20">
+        <v>0.27989999999999998</v>
+      </c>
+      <c r="G66" s="20">
+        <v>6.7299999999999999E-2</v>
+      </c>
+      <c r="H66" s="20">
+        <v>5.8999999999999999E-3</v>
+      </c>
+      <c r="I66" s="20">
+        <v>1E-4</v>
+      </c>
+      <c r="J66" s="21">
+        <v>0.81020000000000003</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update baselines in different criteria
</commit_message>
<xml_diff>
--- a/baselines.xlsx
+++ b/baselines.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quert/Documents/GitHub/KGG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA9C044-086D-1543-A390-7CB09E131244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE48B3DE-9290-FE4C-9130-3C025652DB60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{9DDA97F0-446E-8741-84E0-45819061BEAD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{9DDA97F0-446E-8741-84E0-45819061BEAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="45">
   <si>
     <t>ROUGE-1</t>
   </si>
@@ -140,7 +140,37 @@
     <t>few-shot (modified prompt)</t>
   </si>
   <si>
-    <t>GPTScore</t>
+    <t>similarity - 3.5</t>
+  </si>
+  <si>
+    <t>similarity - 4</t>
+  </si>
+  <si>
+    <t>eval: gpt-4</t>
+  </si>
+  <si>
+    <t>avg</t>
+  </si>
+  <si>
+    <t>reasonable - 3.5</t>
+  </si>
+  <si>
+    <t>reasonable - 4</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>innovation - 3.5</t>
+  </si>
+  <si>
+    <t>innovation - 4</t>
+  </si>
+  <si>
+    <t>valid - 3.5</t>
+  </si>
+  <si>
+    <t>valid - 4</t>
   </si>
 </sst>
 </file>
@@ -152,7 +182,7 @@
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="170" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -172,6 +202,14 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
@@ -233,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -266,22 +304,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -597,21 +639,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21CFAA03-9A7E-9E47-88B5-AB72ED5F4100}">
-  <dimension ref="B1:K75"/>
+  <dimension ref="B1:K104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="K71" sqref="K71"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="144" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="F92" sqref="F92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="3" max="3" width="16.83203125" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" customWidth="1"/>
     <col min="6" max="6" width="17.6640625" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" customWidth="1"/>
+    <col min="10" max="10" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.2">
@@ -2032,9 +2076,7 @@
       <c r="J70" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="K70" s="22" t="s">
-        <v>34</v>
-      </c>
+      <c r="K70" s="22"/>
     </row>
     <row r="71" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B71" s="18" t="s">
@@ -2181,8 +2223,384 @@
         <v>0.81189999999999996</v>
       </c>
     </row>
+    <row r="77" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C77" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D77" s="23"/>
+      <c r="F77" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="G77" s="23"/>
+      <c r="I77" s="23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="78" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C78" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D78" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F78" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="G78" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="I78" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="J78" s="23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="79" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C79">
+        <v>0.25</v>
+      </c>
+      <c r="D79">
+        <v>0.4</v>
+      </c>
+      <c r="F79">
+        <v>0.21</v>
+      </c>
+      <c r="G79">
+        <v>0.45</v>
+      </c>
+      <c r="I79">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="J79">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="80" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C80">
+        <v>0.7</v>
+      </c>
+      <c r="D80">
+        <v>0.6</v>
+      </c>
+      <c r="F80">
+        <v>0.7</v>
+      </c>
+      <c r="G80">
+        <v>0.65</v>
+      </c>
+      <c r="I80">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="J80" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="81" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C81">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="D81">
+        <v>0.3</v>
+      </c>
+      <c r="F81">
+        <v>0.74</v>
+      </c>
+      <c r="G81">
+        <v>0.6</v>
+      </c>
+      <c r="I81">
+        <v>0.6</v>
+      </c>
+      <c r="J81">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="82" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C82">
+        <v>0.65</v>
+      </c>
+      <c r="D82">
+        <v>0.78</v>
+      </c>
+      <c r="F82">
+        <v>0.75</v>
+      </c>
+      <c r="G82">
+        <v>0.5</v>
+      </c>
+      <c r="I82">
+        <v>0.6</v>
+      </c>
+      <c r="J82" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="83" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C83">
+        <v>0.65</v>
+      </c>
+      <c r="D83">
+        <v>0.65</v>
+      </c>
+      <c r="F83">
+        <v>0.75</v>
+      </c>
+      <c r="G83">
+        <v>0.68</v>
+      </c>
+      <c r="I83">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="J83">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="84" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C84">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="D84">
+        <v>0.82920000000000005</v>
+      </c>
+      <c r="F84">
+        <v>0.625</v>
+      </c>
+      <c r="G84">
+        <v>0.65</v>
+      </c>
+      <c r="I84">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="J84">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="85" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C85">
+        <v>0.22</v>
+      </c>
+      <c r="D85">
+        <v>0.25</v>
+      </c>
+      <c r="F85">
+        <v>0.45</v>
+      </c>
+      <c r="G85">
+        <v>0.65</v>
+      </c>
+      <c r="I85">
+        <v>0.6</v>
+      </c>
+      <c r="J85">
+        <v>0.17499999999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C86">
+        <v>0.63</v>
+      </c>
+      <c r="D86">
+        <v>0.65</v>
+      </c>
+      <c r="F86">
+        <v>0.3</v>
+      </c>
+      <c r="G86">
+        <v>0.5</v>
+      </c>
+      <c r="I86">
+        <v>0.67</v>
+      </c>
+      <c r="J86">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="87" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C87">
+        <v>0.7</v>
+      </c>
+      <c r="D87">
+        <v>0.4</v>
+      </c>
+      <c r="F87">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="G87">
+        <v>0.6</v>
+      </c>
+      <c r="I87">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="J87">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="88" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C88">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="D88">
+        <v>0.75</v>
+      </c>
+      <c r="F88">
+        <v>0.875</v>
+      </c>
+      <c r="G88">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="I88">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="J88">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="89" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B89" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C89" s="23">
+        <f>AVERAGE(C79:C88)</f>
+        <v>0.5774999999999999</v>
+      </c>
+      <c r="D89" s="23">
+        <f>AVERAGE(D79:D88)</f>
+        <v>0.56092000000000009</v>
+      </c>
+      <c r="F89" s="23">
+        <f>AVERAGE(F79:F88)</f>
+        <v>0.60749999999999993</v>
+      </c>
+      <c r="G89" s="23">
+        <f>AVERAGE(G79:G88)</f>
+        <v>0.60050000000000003</v>
+      </c>
+      <c r="I89" s="23">
+        <f>AVERAGE(I79:I88)</f>
+        <v>0.59400000000000008</v>
+      </c>
+      <c r="J89" s="23">
+        <f>AVERAGE(J79,J81,J83:J88)</f>
+        <v>0.578125</v>
+      </c>
+    </row>
+    <row r="92" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C92" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D92" s="23"/>
+      <c r="F92" s="23"/>
+      <c r="G92" s="23"/>
+    </row>
+    <row r="93" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C93" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D93" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="F93" s="23"/>
+      <c r="G93" s="23"/>
+    </row>
+    <row r="94" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C94">
+        <v>0.25</v>
+      </c>
+      <c r="D94">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="95" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C95">
+        <v>0.33</v>
+      </c>
+      <c r="D95">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="96" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C97">
+        <v>0.1</v>
+      </c>
+      <c r="D97">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C98">
+        <v>0.6</v>
+      </c>
+      <c r="D98">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C99">
+        <v>0.3</v>
+      </c>
+      <c r="D99">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C100">
+        <v>0.44</v>
+      </c>
+      <c r="D100">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="101" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C101">
+        <v>0.5</v>
+      </c>
+      <c r="D101">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C102">
+        <v>0.4</v>
+      </c>
+      <c r="D102">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="103" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C103">
+        <v>0.15</v>
+      </c>
+      <c r="D103">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="104" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B104" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C104" s="23">
+        <f>AVERAGE(C94:C103)</f>
+        <v>0.307</v>
+      </c>
+      <c r="D104" s="23">
+        <f>AVERAGE(D94:D103)</f>
+        <v>0.3795</v>
+      </c>
+      <c r="E104" s="24"/>
+      <c r="F104" s="23"/>
+      <c r="G104" s="23"/>
+    </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>